<commit_message>
recent changes / update since being idle
</commit_message>
<xml_diff>
--- a/Hardware/FR4_PCB_Mass_vs_Thickness_Estimates.xlsx
+++ b/Hardware/FR4_PCB_Mass_vs_Thickness_Estimates.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanshipley/Documents/Research/2019_ZOE_M8Q_GPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanshipley/Documents/GitHub/Solar_LoRa_GPS/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6723F196-010F-4F47-833B-E69A99A4A273}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A8BEB-3FB7-1E4D-A238-BE942893475E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{303D1030-1C2B-BD44-B662-AE7049AD71C6}"/>
+    <workbookView xWindow="4660" yWindow="1780" windowWidth="25440" windowHeight="14460" xr2:uid="{303D1030-1C2B-BD44-B662-AE7049AD71C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -405,7 +408,7 @@
   <dimension ref="A2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,33 +455,33 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>50.5</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <f>(A5*B5*$G$3)/1000</f>
-        <v>4.2016</v>
+        <v>1.3248000000000002</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="G5">
         <f>(($A5*$B5*$G$3)/1000) * $E5</f>
-        <v>8.4032</v>
+        <v>2.6496000000000004</v>
       </c>
       <c r="H5">
         <f>(($A5*$B5*$H$3)/1000) * $E5</f>
-        <v>4.2016</v>
+        <v>1.3248000000000002</v>
       </c>
       <c r="I5">
         <f>(($A5*$B5*$I$3)/1000) * $E5</f>
-        <v>2.1008</v>
+        <v>0.6624000000000001</v>
       </c>
       <c r="J5">
         <f>(($A5*$B5*$J$3)/1000) * $E5</f>
-        <v>1.0504</v>
+        <v>0.33120000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>